<commit_message>
bento regression 25 scripts
</commit_message>
<xml_diff>
--- a/InputFiles/TC03_Bento_Filter_Chemo-FEC3WkCycles.xlsx
+++ b/InputFiles/TC03_Bento_Filter_Chemo-FEC3WkCycles.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sohilz2\Commons_Automation\InputFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\radhakrishnang2\Desktop\Commons_Automation\InputFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12CA247F-EEF6-4A8F-9961-AEE2B77F5560}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B9EFEB8-9A9C-4D63-A347-E3FED1CAECA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="31530" yWindow="1485" windowWidth="23100" windowHeight="11655" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
   <sheets>
     <sheet name="startup" sheetId="1" r:id="rId1"/>
@@ -102,31 +102,6 @@
   </si>
   <si>
     <t>FilesTab</t>
-  </si>
-  <si>
-    <t>MATCH (ss:study_subject)
-WITH COLLECT(ss.study_subject_id) AS all_subjects
-MATCH (samp:sample)
-MATCH (samp)-[:sample_of_study_subject]-&gt;(ss)
-MATCH (ss)-[:study_subject_of_study]-&gt;(s)-[:study_of_program]-&gt;(p)
-MATCH (samp)&lt;-[:file_of_sample]-(f)-[:file_of_laboratory_procedure]-&gt;(lp)
-MATCH (ss)&lt;-[:diagnosis_of_study_subject]-(d)
-MATCH (d)&lt;-[:tp_of_diagnosis]-(tp)
-WHERE tp.chemotherapy_regimen IN ["FEC (3 week cycles)"]
-    distinct lp,
-    toInteger(split(ss.study_subject_id,'-')[2]) AS subject_id_num,
-    collect(distinct f.file_id) AS files,
-    samp, ss, s, p, all_subjects
-RETURN
- samp.sample_id AS `Sample ID`,
-            ss.study_subject_id AS `Case ID`,
-            p.program_acronym AS `Program Code`,
-            s.study_acronym AS `Arm`,
-            ss.disease_subtype AS `Diagnosis`,
-            samp.tissue_type AS `Tissue Type`,
-            samp.composition AS `Tissue Composition`,
-            samp.sample_anatomic_site AS `Sample Anatomic Site`,
-            samp.method_of_sample_procurement AS `Sample Procurement Method`</t>
   </si>
   <si>
     <t>MATCH (f:file)--&gt;(parent)
@@ -161,6 +136,31 @@
     ss.study_subject_id AS `Case ID`,
     samp.sample_id AS `Sample ID`
     order by f.file_name</t>
+  </si>
+  <si>
+    <t>MATCH (ss:study_subject)
+WITH COLLECT(ss.study_subject_id) AS all_subjects
+MATCH (samp:sample)
+MATCH (samp)-[:sample_of_study_subject]-&gt;(ss)
+MATCH (ss)-[:study_subject_of_study]-&gt;(s)-[:study_of_program]-&gt;(p)
+MATCH (samp)&lt;-[:file_of_sample]-(f)-[:file_of_laboratory_procedure]-&gt;(lp)
+MATCH (ss)&lt;-[:diagnosis_of_study_subject]-(d)
+MATCH (d)&lt;-[:tp_of_diagnosis]-(tp)
+WHERE tp.chemotherapy_regimen IN ["FEC (3 week cycles)"]
+  WITH  distinct lp,
+    toInteger(split(ss.study_subject_id,'-')[2]) AS subject_id_num,
+    collect(distinct f.file_id) AS files,
+    samp, ss, s, p, all_subjects
+RETURN DISTINCT
+ samp.sample_id AS `Sample ID`,
+            ss.study_subject_id AS `Case ID`,
+            p.program_acronym AS `Program Code`,
+            s.study_acronym AS `Arm`,
+            ss.disease_subtype AS `Diagnosis`,
+            samp.tissue_type AS `Tissue Type`,
+            samp.composition AS `Tissue Composition`,
+            samp.sample_anatomic_site AS `Sample Anatomic Site`,
+            samp.method_of_sample_procurement AS `Sample Procurement Method`</t>
   </si>
 </sst>
 </file>
@@ -533,19 +533,19 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="75.88671875" customWidth="1"/>
-    <col min="3" max="3" width="60.44140625" customWidth="1"/>
-    <col min="4" max="4" width="70.33203125" customWidth="1"/>
+    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="75.85546875" customWidth="1"/>
+    <col min="3" max="3" width="60.42578125" customWidth="1"/>
+    <col min="4" max="4" width="70.28515625" customWidth="1"/>
     <col min="5" max="5" width="53" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -562,7 +562,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="316.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" ht="330" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -579,12 +579,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="331.2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" ht="345" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>10</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>8</v>
@@ -596,12 +596,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>11</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>8</v>

</xml_diff>